<commit_message>
Switched to wire antenna XBee to control costs (antennae are expensive!)
</commit_message>
<xml_diff>
--- a/pcb/operator-interface-bom-r1.1.xlsx
+++ b/pcb/operator-interface-bom-r1.1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
   <si>
     <t>Qty</t>
   </si>
@@ -262,9 +262,6 @@
     <t>445-2525-1-ND</t>
   </si>
   <si>
-    <t>Also needs 2 10-pin 2mm headers and an antenna (below)</t>
-  </si>
-  <si>
     <t>2.4 GHz antenna</t>
   </si>
   <si>
@@ -280,18 +277,12 @@
     <t>https://www.adafruit.com/product/366</t>
   </si>
   <si>
-    <t>602-1558-ND</t>
-  </si>
-  <si>
     <t>A24-HASM-450-ND</t>
   </si>
   <si>
     <t>https://www.adafruit.com/product/944</t>
   </si>
   <si>
-    <t>For Xbee. Another alternative is https://www.aliexpress.com/item/FREE-SHIPPING-2pcs-lot-2dbi-Wireless-2-4GHZ-WIFI-Antenna-Female/32810110460.html?spm=2114.search0104.3.38.ZW8tLe&amp;ws_ab_test=searchweb0_0,searchweb201602_1_10152_10065_10151_10344_10068_10130_10345_10342_10547_10343_10340_10341_10548_10541_10084_10083_10139_10307_10178_10060_10155_5640011_10154_5370011_10056_10055_10539_10538_10537_10312_10536_10059_10313_10314_10534_10533_100031_10103_10073_10102_5720011_10142_10107,searchweb201603_1,ppcSwitch_5&amp;btsid=f627d508-4b63-40bc-8a5c-1c198c1cd831&amp;algo_expid=181cd600-c3ef-45f4-9bad-aaff71b5cf67-5&amp;algo_pvid=181cd600-c3ef-45f4-9bad-aaff71b5cf67 - "female" version.</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
@@ -329,6 +320,18 @@
   </si>
   <si>
     <t>S9473CT-ND</t>
+  </si>
+  <si>
+    <t>For Xbee. Only needed if using the RP-SMA Xbee</t>
+  </si>
+  <si>
+    <t>Also needs 2 10-pin 2mm headers and an antenna (below). For more range, use 602-1558-ND instead</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/968</t>
+  </si>
+  <si>
+    <t>602-1560-ND</t>
   </si>
 </sst>
 </file>
@@ -821,11 +824,15 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1181,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1318,11 +1325,11 @@
         <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1330,17 +1337,17 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1348,17 +1355,17 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1492,45 +1499,37 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="2" t="s">
-        <v>82</v>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1538,157 +1537,157 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="3" t="s">
-        <v>87</v>
+      <c r="F17" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>94</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E20" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="F21" s="2" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>11</v>
-      </c>
-      <c r="B23" s="2">
-        <v>330</v>
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E23" s="2"/>
       <c r="F23" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>11</v>
+      </c>
+      <c r="B24" s="2">
+        <v>330</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="F24" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
@@ -1698,44 +1697,64 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>49</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="4" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H27" s="2" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding U1 headers to BOM
</commit_message>
<xml_diff>
--- a/pcb/operator-interface-bom-r1.1.xlsx
+++ b/pcb/operator-interface-bom-r1.1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
   <si>
     <t>Qty</t>
   </si>
@@ -268,12 +268,6 @@
     <t>1528-1392-ND</t>
   </si>
   <si>
-    <t>10-pin 2mm header (pair)</t>
-  </si>
-  <si>
-    <t>For Xbee. Come as a pair.</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/366</t>
   </si>
   <si>
@@ -332,13 +326,55 @@
   </si>
   <si>
     <t>602-1560-ND</t>
+  </si>
+  <si>
+    <t>S7006-ND</t>
+  </si>
+  <si>
+    <t>Also can get a longer header, cut in pieces, and use for this and U1</t>
+  </si>
+  <si>
+    <t>S7012-ND</t>
+  </si>
+  <si>
+    <t>Also can get a longer header, cut in pieces, and use for this and MOD2</t>
+  </si>
+  <si>
+    <t>Socket header for U1</t>
+  </si>
+  <si>
+    <t>Socket header for MOD2</t>
+  </si>
+  <si>
+    <t>Includes 8-pin pin header</t>
+  </si>
+  <si>
+    <t>For Xbee. Come as a pair - only order one pair!</t>
+  </si>
+  <si>
+    <t>10-pin socket 2mm header</t>
+  </si>
+  <si>
+    <t>5-pin pin header for U1</t>
+  </si>
+  <si>
+    <t>S1011EC-05-ND</t>
+  </si>
+  <si>
+    <t>5-pin socket header for U1</t>
+  </si>
+  <si>
+    <t>S6103-ND</t>
+  </si>
+  <si>
+    <t>Also can cut a piece of a longer header</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +508,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -821,16 +863,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1188,15 +1231,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
@@ -1231,530 +1275,594 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>6</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>8</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>6</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="B24" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>2</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>2</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D26" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>11</v>
+      </c>
+      <c r="B27" s="3">
+        <v>330</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>11</v>
-      </c>
-      <c r="B24" s="2">
-        <v>330</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>1</v>
-      </c>
-      <c r="B25" s="2" t="s">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>1</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>1</v>
-      </c>
-      <c r="B26" s="2" t="s">
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>1</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="H29" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>1</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="4" t="s">
+      <c r="E30" s="3"/>
+      <c r="F30" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H30" s="3" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revising some alternate sources
</commit_message>
<xml_diff>
--- a/pcb/operator-interface-bom-r1.1.xlsx
+++ b/pcb/operator-interface-bom-r1.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="operator-interface-display-r1.1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="111">
   <si>
     <t>Qty</t>
   </si>
@@ -61,9 +61,6 @@
     <t>SV2</t>
   </si>
   <si>
-    <t>10u</t>
-  </si>
-  <si>
     <t>CPOL-USE2.5-6</t>
   </si>
   <si>
@@ -169,33 +166,12 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Much cheaper from Aliexpress. Also need joystick cap.</t>
-  </si>
-  <si>
-    <t>Joystick Cap</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Not needed if Joystick includes one</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/3D-Analog-Joystick-Stick-Sensor-Repair-Parts-For-Microsoft-For-Xbox-360-For-PS2-Controller-Joystick/32744295312.html?spm=2114.search0104.3.10.YIwqqZ&amp;ws_ab_test=searchweb0_0,searchweb201602_1_10152_10065_10151_10344_10068_10130_10345_10342_10547_10343_10340_10341_10548_10541_10084_10083_10139_10307_10178_10060_10155_5640011_10154_5370011_10056_10055_10539_10538_10537_10312_10536_10059_10313_10314_10534_10533_100031_10103_10073_10102_5720011_10142_10107,searchweb201603_1,ppcSwitch_5&amp;btsid=da10db06-a55d-4e19-ba11-507ed7700f7d&amp;algo_expid=3cc89f35-19bb-4318-881e-d405c70ba0de-1&amp;algo_pvid=3cc89f35-19bb-4318-881e-d405c70ba0de</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/High-Quality-Analog-3D-Thumb-Sticks-Joystick-Thumbstick-Mushroom-Cap-Cover-For-PS2-Controller-Thumb-Grips/32763331342.html?spm=2114.search0104.3.73.LJbVnk&amp;ws_ab_test=searchweb0_0,searchweb201602_1_10152_10065_10151_10344_10068_10130_10345_10342_10547_10343_10340_10341_10548_10541_10084_10083_10139_10307_10178_10060_10155_5640011_10154_5370011_10056_10055_10539_10538_10537_10312_10536_10059_10313_10314_10534_10533_100031_10103_10073_10102_5720011_10142_10107,searchweb201603_1,ppcSwitch_5&amp;btsid=9a0e423b-ad57-4341-9268-c438ec8125bd&amp;algo_expid=6906629b-d6ff-4fad-8999-3167be9cbc5a-9&amp;algo_pvid=6906629b-d6ff-4fad-8999-3167be9cbc5a</t>
-  </si>
-  <si>
     <t>https://www.adafruit.com/product/938</t>
   </si>
   <si>
     <t>Only needed if you want to charge the battery with the board</t>
   </si>
   <si>
-    <t>https://www.pjrc.com/store/teensy32.html</t>
-  </si>
-  <si>
     <t>Needs to be a Teensy 3.2 - 3.3V regulator on earlier versions isn't powerful enough</t>
   </si>
   <si>
@@ -368,12 +344,21 @@
   </si>
   <si>
     <t>Also can cut a piece of a longer header</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/9032</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/2756 or https://www.pjrc.com/store/teensy32.html</t>
+  </si>
+  <si>
+    <t>10uF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1230,11 +1215,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1259,19 +1244,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1287,7 +1272,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -1305,11 +1290,11 @@
         <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1320,14 +1305,14 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -1337,21 +1322,21 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1369,11 +1354,11 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1381,17 +1366,17 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1399,17 +1384,17 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1417,17 +1402,17 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -1437,23 +1422,23 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1461,17 +1446,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1479,17 +1464,17 @@
         <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1499,21 +1484,21 @@
         <v>1</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1521,20 +1506,20 @@
         <v>1</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H14" s="3"/>
     </row>
@@ -1543,23 +1528,23 @@
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1567,17 +1552,17 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1585,17 +1570,17 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1603,17 +1588,17 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1621,23 +1606,23 @@
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1645,19 +1630,19 @@
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="5"/>
       <c r="F20" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1665,19 +1650,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="5"/>
       <c r="F21" s="4" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1686,14 +1671,14 @@
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1703,19 +1688,19 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -1725,17 +1710,17 @@
         <v>2</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -1746,14 +1731,14 @@
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1763,17 +1748,17 @@
         <v>2</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -1789,13 +1774,13 @@
         <v>8</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1805,17 +1790,17 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1825,46 +1810,22 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>1</v>
-      </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="H29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating LEDs in BOM to white / amber
</commit_message>
<xml_diff>
--- a/pcb/operator-interface-bom-r1.1.xlsx
+++ b/pcb/operator-interface-bom-r1.1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
   <si>
     <t>Qty</t>
   </si>
@@ -253,24 +253,6 @@
     <t>https://www.adafruit.com/product/944</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>C503B-GAN-CC0D0891-ND</t>
-  </si>
-  <si>
-    <t>C503B-RCN-CX0Y0AA1-ND</t>
-  </si>
-  <si>
-    <t>LED7, LED9</t>
-  </si>
-  <si>
-    <t>LED8, LED10</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
     <t>You can also just solder wires to this. Not needed if using a LiPo battery.</t>
   </si>
   <si>
@@ -353,6 +335,18 @@
   </si>
   <si>
     <t>10uF</t>
+  </si>
+  <si>
+    <t>LED7, LED8, LED9, LED10</t>
+  </si>
+  <si>
+    <t>Alternative: C503C-ACN-CYCZA342CT-ND (Amber)</t>
+  </si>
+  <si>
+    <t>Cool White</t>
+  </si>
+  <si>
+    <t>C503C-WAN-CBBDB231-ND</t>
   </si>
 </sst>
 </file>
@@ -1216,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,11 +1348,11 @@
         <v>12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1366,17 +1360,17 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1384,17 +1378,17 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1402,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>13</v>
@@ -1438,7 +1432,7 @@
         <v>48</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1446,17 +1440,17 @@
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1541,7 +1535,7 @@
         <v>67</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>50</v>
@@ -1552,17 +1546,17 @@
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1570,17 +1564,17 @@
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1588,17 +1582,17 @@
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1616,13 +1610,13 @@
         <v>29</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1630,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1642,7 +1636,7 @@
         <v>74</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1662,7 +1656,7 @@
         <v>76</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1685,10 +1679,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>18</v>
@@ -1697,90 +1691,92 @@
         <v>32</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>2</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B24" s="3"/>
       <c r="C24" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
-        <v>80</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="C25" s="3" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>2</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="B26" s="3">
+        <v>330</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F26" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>11</v>
-      </c>
-      <c r="B27" s="3">
-        <v>330</v>
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>15</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -1790,42 +1786,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G28" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>1</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
I jumped the gun on the last update - keyboard has white or amber LEDs, display board has red/green. Fixing.
</commit_message>
<xml_diff>
--- a/pcb/operator-interface-bom-r1.1.xlsx
+++ b/pcb/operator-interface-bom-r1.1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
   <si>
     <t>Qty</t>
   </si>
@@ -337,9 +337,6 @@
     <t>10uF</t>
   </si>
   <si>
-    <t>LED7, LED8, LED9, LED10</t>
-  </si>
-  <si>
     <t>Alternative: C503C-ACN-CYCZA342CT-ND (Amber)</t>
   </si>
   <si>
@@ -347,6 +344,24 @@
   </si>
   <si>
     <t>C503C-WAN-CBBDB231-ND</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>LED8, LED10</t>
+  </si>
+  <si>
+    <t>C503B-GAN-CC0D0891-ND</t>
+  </si>
+  <si>
+    <t>C503B-RCN-CX0Y0AA1-ND</t>
+  </si>
+  <si>
+    <t>LED7, LED9</t>
   </si>
 </sst>
 </file>
@@ -489,13 +504,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -842,19 +858,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1210,10 +1227,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,554 +1271,592 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>2</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>2</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2" t="s">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3" t="s">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>1</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>2</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="2" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="2" t="s">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2" t="s">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>2</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="3" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>1</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="4" t="s">
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>6</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
-        <v>10</v>
-      </c>
-      <c r="B23" s="3" t="s">
+      <c r="A23" s="2">
+        <v>6</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="G23" s="2"/>
+      <c r="H23" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>2</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>2</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>1</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3" t="s">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>2</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>11</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B28" s="2">
         <v>330</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>1</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>1</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H28" s="3"/>
+      <c r="H30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating R12/R13 reference designators on keypad to match the panel file. Includes updates to BOMs.
</commit_message>
<xml_diff>
--- a/pcb/operator-interface-bom-r1.1.xlsx
+++ b/pcb/operator-interface-bom-r1.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
   <si>
     <t>Qty</t>
   </si>
@@ -67,9 +67,6 @@
     <t>C1, C2</t>
   </si>
   <si>
-    <t>R7, R8, R10, R11, R13</t>
-  </si>
-  <si>
     <t>ADAFRUIT-OLED-1.3</t>
   </si>
   <si>
@@ -127,12 +124,6 @@
     <t>10K</t>
   </si>
   <si>
-    <t>R12, R13</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R4, R5, R6</t>
-  </si>
-  <si>
     <t>EG1313</t>
   </si>
   <si>
@@ -151,12 +142,6 @@
     <t>R-US_0207</t>
   </si>
   <si>
-    <t>Reference Designators (keypad)</t>
-  </si>
-  <si>
-    <t>Reference Designators (display)</t>
-  </si>
-  <si>
     <t>Digikey part number</t>
   </si>
   <si>
@@ -362,6 +347,15 @@
   </si>
   <si>
     <t>LED7, LED9</t>
+  </si>
+  <si>
+    <t>R14, R15</t>
+  </si>
+  <si>
+    <t>R1, R2, R3, R4, R5, R6, R7, R8, R10, R11, R13</t>
+  </si>
+  <si>
+    <t>Reference Designators</t>
   </si>
 </sst>
 </file>
@@ -1227,24 +1221,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.28515625" customWidth="1"/>
-    <col min="8" max="8" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.28515625" customWidth="1"/>
+    <col min="7" max="7" width="50.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1255,22 +1248,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1278,17 +1268,16 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1296,19 +1285,18 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -1316,41 +1304,39 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>59</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1360,441 +1346,419 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>63</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>67</v>
+      <c r="E15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>87</v>
+      <c r="E19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3" t="s">
-        <v>75</v>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>6</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="E22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>112</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="E26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2" t="s">
-        <v>58</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>11</v>
       </c>
@@ -1805,58 +1769,53 @@
         <v>8</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>57</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2" t="s">
-        <v>56</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="F30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H30" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="G30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>